<commit_message>
Final, 200th commit. I am submitting now.
</commit_message>
<xml_diff>
--- a/Documentation/gantt-chart.xlsx
+++ b/Documentation/gantt-chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10806"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cruz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Desktop/DOCUMENTATION/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC2A38A-E0BF-C841-8BC1-0E2443B73C06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15520" windowHeight="7790"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="15520" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -585,23 +586,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -627,7 +629,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -641,7 +643,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -657,7 +659,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>10</v>
@@ -671,7 +673,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>11</v>
@@ -685,7 +687,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -701,7 +703,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>14</v>
@@ -715,7 +717,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -731,7 +733,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -745,7 +747,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -759,7 +761,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -773,7 +775,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
@@ -789,7 +791,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16"/>
       <c r="B13" s="13" t="s">
         <v>20</v>
@@ -803,7 +805,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
@@ -817,7 +819,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
@@ -831,7 +833,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -845,7 +847,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -858,7 +860,7 @@
       <c r="J17" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>